<commit_message>
Added chapter about cell contents, Typos removed
</commit_message>
<xml_diff>
--- a/tutorial/samplefile.xlsx
+++ b/tutorial/samplefile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a.hanisch/Sources/xlsx-tutorial/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/armin/sourcecode/go-modules/xlsx/tutorial/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56E0530-0E0D-9A4F-BB52-71CCA80E589D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E397043E-32BE-9F42-AB67-FF79EC6A1726}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="460" windowWidth="24940" windowHeight="14980" activeTab="1" xr2:uid="{E70933EE-B250-8A41-96D6-CFCBFBE01D85}"/>
+    <workbookView xWindow="720" yWindow="460" windowWidth="24940" windowHeight="14980" xr2:uid="{E70933EE-B250-8A41-96D6-CFCBFBE01D85}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample" sheetId="1" r:id="rId1"/>
@@ -115,7 +115,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -134,6 +134,14 @@
     <font>
       <sz val="12"/>
       <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -162,10 +170,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -182,8 +191,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -498,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1FA3B21-DAC7-1346-9A97-5BE17C6C1F69}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -522,7 +535,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4">
@@ -537,7 +550,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="4">
@@ -567,10 +580,12 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" location="cities" tooltip="Links to the cities range" display="Alice" xr:uid="{D752B12A-2FFB-B74D-9623-1A1AC7FF1792}"/>
+    <hyperlink ref="A3" r:id="rId1" tooltip="The Joy of Painting" xr:uid="{F334C42A-9A70-9641-BA0A-28C097A6CA6B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddFooter>&amp;R_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;I0000FF Classification: EMG Internal</oddFooter>
-  </headerFooter>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -578,7 +593,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F8D1768-D68C-4349-B4EE-53C43024E9EA}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>

</xml_diff>